<commit_message>
Added second sensor outside the court. Given the physical condition is on separate pin
</commit_message>
<xml_diff>
--- a/Connector labels.xlsx
+++ b/Connector labels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\petla\Documents\PlatformIO\Projects\WeatherSensorsSigiFox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE1044E-7EEB-4544-88E3-7F1F6D38A947}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3AE1AD-BAA7-4CB2-9F10-727EC34130DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{8A9B3727-6D6B-4D2F-B2F1-C365EB0F93ED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8A9B3727-6D6B-4D2F-B2F1-C365EB0F93ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>5V</t>
   </si>
@@ -82,7 +82,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,14 +114,6 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color theme="0"/>
-      <name val="Symbol"/>
-      <family val="1"/>
-      <charset val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -215,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -230,10 +222,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -248,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -565,20 +554,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358FDF87-2423-431A-BA6D-0BBF7AF7439F}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="175" zoomScaleNormal="100" zoomScalePageLayoutView="175" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="17" width="2.7109375" customWidth="1"/>
+    <col min="1" max="17" width="2.6640625" customWidth="1"/>
     <col min="18" max="18" width="3" customWidth="1"/>
-    <col min="19" max="19" width="3.5703125" customWidth="1"/>
+    <col min="19" max="19" width="3.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -605,18 +594,18 @@
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>5</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="9"/>
-      <c r="P1" s="10" t="s">
+      <c r="O1" s="8"/>
+      <c r="P1" s="9" t="s">
         <v>16</v>
       </c>
       <c r="Q1" s="1"/>
@@ -625,7 +614,7 @@
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -643,17 +632,17 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -680,18 +669,44 @@
       <c r="L3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
     </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed bugs with reading sensor and labeling connectors
</commit_message>
<xml_diff>
--- a/Connector labels.xlsx
+++ b/Connector labels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\petla\Documents\PlatformIO\Projects\WeatherSensorsSigiFox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3AE1AD-BAA7-4CB2-9F10-727EC34130DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E5F3B4-D021-4DD4-82FD-4F2C3A4409FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8A9B3727-6D6B-4D2F-B2F1-C365EB0F93ED}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{8A9B3727-6D6B-4D2F-B2F1-C365EB0F93ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Rx</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
     <t>D2</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>D7</t>
   </si>
 </sst>
 </file>
@@ -557,7 +557,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="175" zoomScaleNormal="100" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,7 +594,7 @@
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K1" s="11" t="s">
         <v>5</v>
@@ -602,11 +602,11 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O1" s="8"/>
       <c r="P1" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="1"/>
       <c r="R1" s="2"/>
@@ -667,7 +667,7 @@
         <v>12</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>

</xml_diff>